<commit_message>
TUM Lite Enchanted 1.3
Rebalance Creatures
</commit_message>
<xml_diff>
--- a/TUM Lite Enchanted/Data/s/Creatures Cost TUM Lite Enchanted Edition.xlsx
+++ b/TUM Lite Enchanted/Data/s/Creatures Cost TUM Lite Enchanted Edition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -583,7 +583,7 @@
         <v>19900</v>
       </c>
       <c r="I6" s="1">
-        <v>17090</v>
+        <v>17030</v>
       </c>
       <c r="J6" s="1">
         <v>17380</v>
@@ -593,7 +593,7 @@
       </c>
       <c r="L6">
         <f>C6+D6+E6+F6+G6+H6+I6+J6+K6</f>
-        <v>167384</v>
+        <v>167324</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>1</v>
@@ -959,17 +959,17 @@
         <v>29300</v>
       </c>
       <c r="I17" s="1">
-        <v>25950</v>
+        <v>25790</v>
       </c>
       <c r="J17" s="1">
-        <v>24420</v>
+        <v>23900</v>
       </c>
       <c r="K17" s="1">
         <v>29440</v>
       </c>
       <c r="L17">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17</f>
-        <v>242179</v>
+        <v>241499</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
@@ -1172,8 +1172,8 @@
         <v>1</v>
       </c>
       <c r="C28" s="1">
-        <f>(150*20)+(200*16)+(290*15)+(500*8)+(550*6)+(2000*4)+(10000*2)</f>
-        <v>45850</v>
+        <f>(150*20)+(200*16)+(290*13)+(500*8)+(550*6)+(2000*4)+(10000*2)</f>
+        <v>45270</v>
       </c>
       <c r="D28" s="1">
         <f>(180*20)+(290*15)+(400*12)+(350*10)+(650*8)+(1500*4)+(8500*2)</f>
@@ -1196,12 +1196,12 @@
         <v>46105</v>
       </c>
       <c r="I28" s="1">
-        <f>(90*38)+(220*22)+(320*18)+(550*8)+(765*6)+(2200*4)+(7600*2)</f>
-        <v>47010</v>
+        <f>(85*38)+(200*22)+(310*18)+(520*8)+(755*6)+(2000*4)+(7400*2)</f>
+        <v>44700</v>
       </c>
       <c r="J28" s="1">
-        <f>(130*28)+(230*20)+(330*16)+(450*8)+(890*6)+(1860*4)+(8100*2)</f>
-        <v>46100</v>
+        <f>(110*28)+(230*20)+(330*16)+(450*8)+(890*6)+(1860*4)+(8000*2)</f>
+        <v>45340</v>
       </c>
       <c r="K28" s="1">
         <f>(60*50)+(350*14)+(500*14)+(500*14)+(680*10)+(1800*4)+(5000*2)</f>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="L28">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28</f>
-        <v>412101</v>
+        <v>408451</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>